<commit_message>
added comp2 files, updated data for ohms law lab
</commit_message>
<xml_diff>
--- a/ohm/PHY224 Ohm Lab.xlsx
+++ b/ohm/PHY224 Ohm Lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/js/school/phy224/ohm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D0602B-70C6-034C-86C7-D804DBC03823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B4FFEF-194C-F34E-8AED-1D0873BBF9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="2300" windowWidth="28800" windowHeight="17540" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Reading</t>
   </si>
   <si>
-    <t>200 Ohms</t>
-  </si>
-  <si>
     <t>2 kOhms</t>
   </si>
   <si>
@@ -140,16 +137,29 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>200 kOhms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -185,6 +195,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,19 +515,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1FA504-BF5F-6343-8346-DC2B6EE3C439}">
-  <dimension ref="A1:AH45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1.373</v>
       </c>
@@ -555,21 +572,22 @@
         <f>MAX(IF(E2=2, 0.001, IF(E2=20, 0.01, IF(E2=200, 0.1))), 0.0025*D2)</f>
         <v>2.8050000000000002E-3</v>
       </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G11" si="0">A2*1000/D2</f>
-        <v>1223.7076648841353</v>
-      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G10" si="0">D2/(A2/1000)</f>
+        <v>817.18863801893667</v>
+      </c>
+      <c r="H2" s="3"/>
       <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
       <c r="R2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>3.81</v>
       </c>
@@ -577,7 +595,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C44" si="1">MAX(IF(B3=2, 0.001, IF(B3=20, 0.01, IF(B3=200, 0.1))), 0.0075*A3)</f>
+        <f t="shared" ref="C3:C11" si="1">MAX(IF(B3=2, 0.001, IF(B3=20, 0.01, IF(B3=200, 0.1))), 0.0075*A3)</f>
         <v>2.8575E-2</v>
       </c>
       <c r="D3" s="2">
@@ -587,13 +605,14 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F44" si="2">MAX(IF(E3=2, 0.001, IF(E3=20, 0.01, IF(E3=200, 0.1))), 0.0025*D3)</f>
+        <f t="shared" ref="F3:F11" si="2">MAX(IF(E3=2, 0.001, IF(E3=20, 0.01, IF(E3=200, 0.1))), 0.0025*D3)</f>
         <v>0.01</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="8">
         <f t="shared" si="0"/>
-        <v>1225.0803858520901</v>
-      </c>
+        <v>816.27296587926503</v>
+      </c>
+      <c r="H3" s="7"/>
       <c r="I3" t="s">
         <v>15</v>
       </c>
@@ -613,7 +632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -634,21 +653,22 @@
         <f t="shared" si="2"/>
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="8">
         <f t="shared" si="0"/>
-        <v>1230.46875</v>
-      </c>
+        <v>812.69841269841265</v>
+      </c>
+      <c r="H4" s="6"/>
       <c r="I4">
         <f>AVERAGE(G2:G11)</f>
-        <v>1230.4499338030441</v>
+        <v>812.71926137311004</v>
       </c>
       <c r="J4">
         <f>STDEV(G2:G11)</f>
-        <v>4.175093708179606</v>
+        <v>2.7574731923806293</v>
       </c>
       <c r="K4">
         <f>J4/COUNT(G2:G11)</f>
-        <v>0.41750937081796058</v>
+        <v>0.27574731923806295</v>
       </c>
       <c r="P4" s="2">
         <v>3.81</v>
@@ -660,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>6.82</v>
       </c>
@@ -681,10 +701,11 @@
         <f t="shared" si="2"/>
         <v>1.3825E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>1233.2730560578661</v>
-      </c>
+        <v>810.85043988269797</v>
+      </c>
+      <c r="H5" s="6"/>
       <c r="P5" s="2" t="s">
         <v>4</v>
       </c>
@@ -695,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>9.36</v>
       </c>
@@ -716,10 +737,11 @@
         <f t="shared" si="2"/>
         <v>1.9E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="8">
         <f t="shared" si="0"/>
-        <v>1231.578947368421</v>
-      </c>
+        <v>811.96581196581189</v>
+      </c>
+      <c r="H6" s="6"/>
       <c r="J6" t="s">
         <v>18</v>
       </c>
@@ -736,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>9.49</v>
       </c>
@@ -757,10 +779,11 @@
         <f t="shared" si="2"/>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>1229.2746113989638</v>
-      </c>
+        <v>813.48788198103261</v>
+      </c>
+      <c r="H7" s="6"/>
       <c r="I7" t="s">
         <v>29</v>
       </c>
@@ -783,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>14.22</v>
       </c>
@@ -804,15 +827,16 @@
         <f t="shared" si="2"/>
         <v>2.8900000000000002E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>1230.1038062283737</v>
-      </c>
+        <v>812.93952180028134</v>
+      </c>
+      <c r="H8" s="6"/>
       <c r="I8" t="s">
         <v>28</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8">
         <v>10</v>
@@ -830,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>15.57</v>
       </c>
@@ -851,10 +875,11 @@
         <f t="shared" si="2"/>
         <v>3.1675000000000002E-2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
-        <v>1228.887134964483</v>
-      </c>
+        <v>813.74438021836863</v>
+      </c>
+      <c r="H9" s="6"/>
       <c r="I9" t="s">
         <v>27</v>
       </c>
@@ -879,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>17.07</v>
       </c>
@@ -900,10 +925,11 @@
         <f t="shared" si="2"/>
         <v>3.4575000000000002E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>1234.2733188720174</v>
-      </c>
+        <v>810.19332161687157</v>
+      </c>
+      <c r="H10" s="6"/>
       <c r="I10" t="s">
         <v>26</v>
       </c>
@@ -927,32 +953,8 @@
       <c r="R10">
         <v>1</v>
       </c>
-      <c r="W10" s="2">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="X10">
-        <v>2</v>
-      </c>
-      <c r="Y10" s="4">
-        <f>MAX(IF(X10=2, 0.001, IF(X10=20, 0.01, IF(X10=200, 0.1))), 0.0075*W10)</f>
-        <v>3.885E-3</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>4.34</v>
-      </c>
-      <c r="AA10">
-        <v>20</v>
-      </c>
-      <c r="AB10">
-        <f>MAX(IF(AA10=2, 0.001, IF(AA10=20, 0.01, IF(AA10=200, 0.1))), 0.0025*Z10)</f>
-        <v>1.085E-2</v>
-      </c>
-      <c r="AC10" s="1">
-        <f t="shared" ref="AC10:AC19" si="3">W10*1000/Z10</f>
-        <v>119.35483870967742</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>19.36</v>
       </c>
@@ -973,10 +975,11 @@
         <f t="shared" si="2"/>
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" si="0"/>
-        <v>1237.8516624040919</v>
-      </c>
+      <c r="G11" s="8">
+        <f t="shared" ref="G11:G21" si="3">D11/(A11/1000)</f>
+        <v>807.8512396694216</v>
+      </c>
+      <c r="H11" s="6"/>
       <c r="P11" s="2">
         <v>17.07</v>
       </c>
@@ -986,41 +989,8 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="W11" s="2">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="X11">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="4">
-        <f>MAX(IF(X11=2, 0.001, IF(X11=20, 0.01, IF(X11=200, 0.1))), 0.0075*W11)</f>
-        <v>5.0625000000000002E-3</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>5.58</v>
-      </c>
-      <c r="AA11">
-        <v>20</v>
-      </c>
-      <c r="AB11">
-        <f>MAX(IF(AA11=2, 0.001, IF(AA11=20, 0.01, IF(AA11=200, 0.1))), 0.0025*Z11)</f>
-        <v>1.3950000000000001E-2</v>
-      </c>
-      <c r="AC11" s="1">
-        <f t="shared" si="3"/>
-        <v>120.96774193548387</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
@@ -1034,311 +1004,375 @@
       <c r="R12">
         <v>1</v>
       </c>
-      <c r="W12" s="2">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="X12">
-        <v>2</v>
-      </c>
-      <c r="Y12" s="4">
-        <f>MAX(IF(X12=2, 0.001, IF(X12=20, 0.01, IF(X12=200, 0.1))), 0.0075*W12)</f>
-        <v>5.8875000000000004E-3</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>6.49</v>
-      </c>
-      <c r="AA12">
-        <v>20</v>
-      </c>
-      <c r="AB12">
-        <f>MAX(IF(AA12=2, 0.001, IF(AA12=20, 0.01, IF(AA12=200, 0.1))), 0.0025*Z12)</f>
-        <v>1.6225E-2</v>
-      </c>
-      <c r="AC12" s="2">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <f>MAX(IF(B13=2, 0.001, IF(B13=20, 0.01, IF(B13=200, 0.1))), 0.0075*A13)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <f>MAX(IF(E13=2, 0.001, IF(E13=20, 0.01, IF(E13=200, 0.1))), 0.0025*D13)</f>
+        <v>1.1050000000000001E-2</v>
+      </c>
+      <c r="G13" s="8">
         <f t="shared" si="3"/>
-        <v>120.9553158705701</v>
-      </c>
-      <c r="AD12" s="3"/>
-      <c r="AE12">
-        <f>AVERAGE(AC10:AC19)</f>
-        <v>120.77282306973936</v>
-      </c>
-      <c r="AF12">
-        <f>STDEV(AC10:AC19)</f>
-        <v>0.50579740382961835</v>
-      </c>
-      <c r="AG12">
-        <f>AF12/COUNT(AC10:AC19)</f>
-        <v>5.0579740382961834E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33740.45801526717</v>
+      </c>
+      <c r="H13" s="3"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="W13" s="2">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="X13">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="4">
-        <f>MAX(IF(X13=2, 0.001, IF(X13=20, 0.01, IF(X13=200, 0.1))), 0.0075*W13)</f>
-        <v>6.9449999999999998E-3</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>7.65</v>
-      </c>
-      <c r="AA13">
-        <v>20</v>
-      </c>
-      <c r="AB13">
-        <f>MAX(IF(AA13=2, 0.001, IF(AA13=20, 0.01, IF(AA13=200, 0.1))), 0.0025*Z13)</f>
-        <v>1.9125E-2</v>
-      </c>
-      <c r="AC13" s="1">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <f>MAX(IF(B14=2, 0.001, IF(B14=20, 0.01, IF(B14=200, 0.1))), 0.0075*A14)</f>
+        <v>1.2750000000000001E-3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.57</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <f>MAX(IF(E14=2, 0.001, IF(E14=20, 0.01, IF(E14=200, 0.1))), 0.0025*D14)</f>
+        <v>1.3925000000000002E-2</v>
+      </c>
+      <c r="G14" s="8">
         <f t="shared" si="3"/>
-        <v>121.04575163398692</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+        <v>32764.705882352941</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="W14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="X14">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="4">
-        <f>MAX(IF(X14=2, 0.001, IF(X14=20, 0.01, IF(X14=200, 0.1))), 0.0075*W14)</f>
-        <v>7.9500000000000005E-3</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>8.77</v>
-      </c>
-      <c r="AA14">
-        <v>20</v>
-      </c>
-      <c r="AB14">
-        <f>MAX(IF(AA14=2, 0.001, IF(AA14=20, 0.01, IF(AA14=200, 0.1))), 0.0025*Z14)</f>
-        <v>2.1925E-2</v>
-      </c>
-      <c r="AC14" s="1">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>0.187</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <f>MAX(IF(B15=2, 0.001, IF(B15=20, 0.01, IF(B15=200, 0.1))), 0.0075*A15)</f>
+        <v>1.4024999999999999E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <f>MAX(IF(E15=2, 0.001, IF(E15=20, 0.01, IF(E15=200, 0.1))), 0.0025*D15)</f>
+        <v>1.5575000000000002E-2</v>
+      </c>
+      <c r="G15" s="8">
         <f t="shared" si="3"/>
-        <v>120.86659064994299</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33315.508021390378</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15">
+        <f>AVERAGE(G13:G22)</f>
+        <v>33384.608442451325</v>
+      </c>
+      <c r="J15">
+        <f>STDEV(G13:G22)</f>
+        <v>246.83250186969232</v>
+      </c>
+      <c r="K15">
+        <f>J15/COUNT(G13:G22)</f>
+        <v>24.683250186969232</v>
+      </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="W15" s="2">
-        <v>1.3819999999999999</v>
-      </c>
-      <c r="X15">
-        <v>2</v>
-      </c>
-      <c r="Y15" s="4">
-        <f>MAX(IF(X15=2, 0.001, IF(X15=20, 0.01, IF(X15=200, 0.1))), 0.0075*W15)</f>
-        <v>1.0364999999999999E-2</v>
-      </c>
-      <c r="Z15" s="2">
-        <v>11.43</v>
-      </c>
-      <c r="AA15">
-        <v>20</v>
-      </c>
-      <c r="AB15">
-        <f>MAX(IF(AA15=2, 0.001, IF(AA15=20, 0.01, IF(AA15=200, 0.1))), 0.0025*Z15)</f>
-        <v>2.8575E-2</v>
-      </c>
-      <c r="AC15" s="1">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <f>MAX(IF(B16=2, 0.001, IF(B16=20, 0.01, IF(B16=200, 0.1))), 0.0075*A16)</f>
+        <v>1.74E-3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.74</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <f>MAX(IF(E16=2, 0.001, IF(E16=20, 0.01, IF(E16=200, 0.1))), 0.0025*D16)</f>
+        <v>1.9350000000000003E-2</v>
+      </c>
+      <c r="G16" s="8">
         <f t="shared" si="3"/>
-        <v>120.90988626421698</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF15">
-        <v>8.27</v>
-      </c>
-      <c r="AG15">
-        <v>83</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33362.068965517239</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="W16" s="2">
-        <v>1.448</v>
-      </c>
-      <c r="X16">
-        <v>2</v>
-      </c>
-      <c r="Y16" s="4">
-        <f>MAX(IF(X16=2, 0.001, IF(X16=20, 0.01, IF(X16=200, 0.1))), 0.0075*W16)</f>
-        <v>1.086E-2</v>
-      </c>
-      <c r="Z16" s="2">
-        <v>11.97</v>
-      </c>
-      <c r="AA16">
-        <v>20</v>
-      </c>
-      <c r="AB16">
-        <f>MAX(IF(AA16=2, 0.001, IF(AA16=20, 0.01, IF(AA16=200, 0.1))), 0.0025*Z16)</f>
-        <v>2.9925000000000004E-2</v>
-      </c>
-      <c r="AC16" s="1">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <f>MAX(IF(B17=2, 0.001, IF(B17=20, 0.01, IF(B17=200, 0.1))), 0.0075*A17)</f>
+        <v>2.2575E-3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>10.06</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <f>MAX(IF(E17=2, 0.001, IF(E17=20, 0.01, IF(E17=200, 0.1))), 0.0025*D17)</f>
+        <v>2.5150000000000002E-2</v>
+      </c>
+      <c r="G17" s="8">
         <f t="shared" si="3"/>
-        <v>120.96908939014202</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF16">
-        <v>20</v>
-      </c>
-      <c r="AG16">
-        <v>100</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33421.926910299007</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="W17" s="2">
-        <v>1.6659999999999999</v>
-      </c>
-      <c r="X17">
-        <v>2</v>
-      </c>
-      <c r="Y17" s="4">
-        <f>MAX(IF(X17=2, 0.001, IF(X17=20, 0.01, IF(X17=200, 0.1))), 0.0075*W17)</f>
-        <v>1.2494999999999999E-2</v>
-      </c>
-      <c r="Z17" s="2">
-        <v>13.78</v>
-      </c>
-      <c r="AA17">
-        <v>20</v>
-      </c>
-      <c r="AB17">
-        <f>MAX(IF(AA17=2, 0.001, IF(AA17=20, 0.01, IF(AA17=200, 0.1))), 0.0025*Z17)</f>
-        <v>3.4450000000000001E-2</v>
-      </c>
-      <c r="AC17" s="1">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
+        <f>MAX(IF(B18=2, 0.001, IF(B18=20, 0.01, IF(B18=200, 0.1))), 0.0075*A18)</f>
+        <v>2.5874999999999995E-3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>11.54</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <f>MAX(IF(E18=2, 0.001, IF(E18=20, 0.01, IF(E18=200, 0.1))), 0.0025*D18)</f>
+        <v>2.8849999999999997E-2</v>
+      </c>
+      <c r="G18" s="8">
         <f t="shared" si="3"/>
-        <v>120.89985486211901</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF17">
-        <f>AF15*1000</f>
-        <v>8270</v>
-      </c>
-      <c r="AG17">
-        <f>AG15*AG16</f>
-        <v>8300</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33449.27536231884</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18">
+        <v>33.4</v>
+      </c>
+      <c r="K18">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="W18" s="2">
-        <v>1.869</v>
-      </c>
-      <c r="X18">
-        <v>2</v>
-      </c>
-      <c r="Y18" s="4">
-        <f>MAX(IF(X18=2, 0.001, IF(X18=20, 0.01, IF(X18=200, 0.1))), 0.0075*W18)</f>
-        <v>1.4017499999999999E-2</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>15.48</v>
-      </c>
-      <c r="AA18">
-        <v>20</v>
-      </c>
-      <c r="AB18">
-        <f>MAX(IF(AA18=2, 0.001, IF(AA18=20, 0.01, IF(AA18=200, 0.1))), 0.0025*Z18)</f>
-        <v>3.8700000000000005E-2</v>
-      </c>
-      <c r="AC18" s="1">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4">
+        <f>MAX(IF(B19=2, 0.001, IF(B19=20, 0.01, IF(B19=200, 0.1))), 0.0075*A19)</f>
+        <v>3.0075000000000002E-3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>13.41</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <f>MAX(IF(E19=2, 0.001, IF(E19=20, 0.01, IF(E19=200, 0.1))), 0.0025*D19)</f>
+        <v>3.3524999999999999E-2</v>
+      </c>
+      <c r="G19" s="8">
         <f t="shared" si="3"/>
-        <v>120.73643410852713</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF18">
-        <f>MAX(0.01*1000,IF(AF16=200,0.005*AF17,0.002*AF17))</f>
-        <v>16.54</v>
-      </c>
-      <c r="AG18">
-        <f>0.05*AG17</f>
-        <v>415</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33441.396508728176</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19">
+        <v>1000</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="W19" s="2">
-        <v>2.13</v>
-      </c>
-      <c r="X19">
-        <v>20</v>
-      </c>
-      <c r="Y19" s="4">
-        <f>MAX(IF(X19=2, 0.001, IF(X19=20, 0.01, IF(X19=200, 0.1))), 0.0075*W19)</f>
-        <v>1.5975E-2</v>
-      </c>
-      <c r="Z19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA19">
-        <v>20</v>
-      </c>
-      <c r="AB19">
-        <f>MAX(IF(AA19=2, 0.001, IF(AA19=20, 0.01, IF(AA19=200, 0.1))), 0.0025*Z19)</f>
-        <v>4.4000000000000004E-2</v>
-      </c>
-      <c r="AC19" s="1">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4">
+        <f>MAX(IF(B20=2, 0.001, IF(B20=20, 0.01, IF(B20=200, 0.1))), 0.0075*A20)</f>
+        <v>3.4199999999999999E-3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>15.23</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <f>MAX(IF(E20=2, 0.001, IF(E20=20, 0.01, IF(E20=200, 0.1))), 0.0025*D20)</f>
+        <v>3.8075000000000005E-2</v>
+      </c>
+      <c r="G20" s="8">
         <f t="shared" si="3"/>
-        <v>121.02272727272727</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+        <v>33399.122807017542</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20">
+        <v>33400</v>
+      </c>
+      <c r="K20">
+        <v>33000</v>
+      </c>
+      <c r="L20" t="s">
+        <v>34</v>
+      </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4">
+        <f>MAX(IF(B21=2, 0.001, IF(B21=20, 0.01, IF(B21=200, 0.1))), 0.0075*A21)</f>
+        <v>3.885E-3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>17.37</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f>MAX(IF(E21=2, 0.001, IF(E21=20, 0.01, IF(E21=200, 0.1))), 0.0025*D21)</f>
+        <v>4.3425000000000005E-2</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="3"/>
+        <v>33532.818532818535</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21">
+        <f>MAX(0.1*1,IF(J19=200,0.005*J20,0.002*J20))</f>
+        <v>66.8</v>
+      </c>
+      <c r="K21">
+        <f>0.05*K20</f>
+        <v>1650</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4">
+        <f>MAX(IF(B22=2, 0.001, IF(B22=20, 0.01, IF(B22=200, 0.1))), 0.0075*A22)</f>
+        <v>4.3874999999999999E-3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>19.55</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f>MAX(IF(E22=2, 0.001, IF(E22=20, 0.01, IF(E22=200, 0.1))), 0.0025*D22)</f>
+        <v>4.8875000000000002E-2</v>
+      </c>
+      <c r="G22" s="8">
+        <f>D22/(A22/1000)</f>
+        <v>33418.803418803422</v>
+      </c>
+      <c r="H22" s="3"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
@@ -1353,30 +1387,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>0.13100000000000001</v>
+        <v>1.96</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <f>MAX(IF(B24=2, 0.001, IF(B24=20, 0.01, IF(B24=200, 0.1))), 0.0075*A24)</f>
+        <v>1.47E-2</v>
       </c>
       <c r="D24" s="2">
-        <v>4.42</v>
+        <v>1.33</v>
       </c>
       <c r="E24">
         <v>20</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
-        <v>1.1050000000000001E-2</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" ref="G24:G33" si="4">A24*1000/D24</f>
-        <v>29.638009049773757</v>
+        <f>MAX(IF(E24=2, 0.001, IF(E24=20, 0.01, IF(E24=200, 0.1))), 0.0025*D24)</f>
+        <v>0.01</v>
+      </c>
+      <c r="G24" s="8">
+        <f>D24/(A24/1000)</f>
+        <v>678.57142857142867</v>
       </c>
       <c r="H24" s="3"/>
       <c r="P24" s="2" t="s">
@@ -1389,31 +1423,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>7.34</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" si="1"/>
-        <v>1.2750000000000001E-3</v>
+        <f>MAX(IF(B25=2, 0.001, IF(B25=20, 0.01, IF(B25=200, 0.1))), 0.0075*A25)</f>
+        <v>5.5049999999999995E-2</v>
       </c>
       <c r="D25" s="2">
-        <v>5.57</v>
+        <v>4.96</v>
       </c>
       <c r="E25">
         <v>20</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
-        <v>1.3925000000000002E-2</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="4"/>
-        <v>30.520646319569117</v>
-      </c>
+        <f>MAX(IF(E25=2, 0.001, IF(E25=20, 0.01, IF(E25=200, 0.1))), 0.0025*D25)</f>
+        <v>1.24E-2</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" ref="G25:G44" si="4">D25/(A25/1000)</f>
+        <v>675.74931880108988</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" t="s">
         <v>15</v>
       </c>
@@ -1433,42 +1468,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>0.187</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="1"/>
-        <v>1.4024999999999999E-3</v>
-      </c>
-      <c r="D26" s="2">
-        <v>6.23</v>
+        <f>MAX(IF(B26=2, 0.001, IF(B26=20, 0.01, IF(B26=200, 0.1))), 0.0075*A26)</f>
+        <v>6.1650000000000003E-2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E26">
         <v>20</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>1.5575000000000002E-2</v>
-      </c>
-      <c r="G26" s="1">
+        <f>MAX(IF(E26=2, 0.001, IF(E26=20, 0.01, IF(E26=200, 0.1))), 0.0025*D26)</f>
+        <v>1.375E-2</v>
+      </c>
+      <c r="G26" s="8">
         <f t="shared" si="4"/>
-        <v>30.016051364365968</v>
-      </c>
+        <v>669.09975669099754</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26">
         <f>AVERAGE(G24:G33)</f>
-        <v>29.955412650185156</v>
+        <v>673.09717479180927</v>
       </c>
       <c r="J26">
         <f>STDEV(G24:G33)</f>
-        <v>0.22383525620483971</v>
+        <v>3.2541604809105023</v>
       </c>
       <c r="K26">
         <f>J26/COUNT(G24:G33)</f>
-        <v>2.2383525620483971E-2</v>
+        <v>0.32541604809105024</v>
       </c>
       <c r="P26" s="2">
         <v>0.23200000000000001</v>
@@ -1480,31 +1516,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>0.23200000000000001</v>
+        <v>10.77</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" si="1"/>
-        <v>1.74E-3</v>
+        <f>MAX(IF(B27=2, 0.001, IF(B27=20, 0.01, IF(B27=200, 0.1))), 0.0075*A27)</f>
+        <v>8.0775E-2</v>
       </c>
       <c r="D27" s="2">
-        <v>7.74</v>
+        <v>7.27</v>
       </c>
       <c r="E27">
         <v>20</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
-        <v>1.9350000000000003E-2</v>
-      </c>
-      <c r="G27" s="1">
+        <f>MAX(IF(E27=2, 0.001, IF(E27=20, 0.01, IF(E27=200, 0.1))), 0.0025*D27)</f>
+        <v>1.8175E-2</v>
+      </c>
+      <c r="G27" s="8">
         <f t="shared" si="4"/>
-        <v>29.974160206718345</v>
-      </c>
+        <v>675.02321262766941</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="P27" s="2">
         <v>0.30099999999999999</v>
       </c>
@@ -1515,31 +1552,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>0.30099999999999999</v>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" si="1"/>
-        <v>2.2575E-3</v>
+        <f>MAX(IF(B28=2, 0.001, IF(B28=20, 0.01, IF(B28=200, 0.1))), 0.0075*A28)</f>
+        <v>8.6249999999999993E-2</v>
       </c>
       <c r="D28" s="2">
-        <v>10.06</v>
+        <v>7.76</v>
       </c>
       <c r="E28">
         <v>20</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
-        <v>2.5150000000000002E-2</v>
-      </c>
-      <c r="G28" s="1">
+        <f>MAX(IF(E28=2, 0.001, IF(E28=20, 0.01, IF(E28=200, 0.1))), 0.0025*D28)</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="G28" s="8">
         <f t="shared" si="4"/>
-        <v>29.920477137176938</v>
-      </c>
+        <v>674.78260869565213</v>
+      </c>
+      <c r="H28" s="5"/>
       <c r="J28" t="s">
         <v>18</v>
       </c>
@@ -1556,42 +1594,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>0.34499999999999997</v>
+        <v>14.35</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" si="1"/>
-        <v>2.5874999999999995E-3</v>
+        <f>MAX(IF(B29=2, 0.001, IF(B29=20, 0.01, IF(B29=200, 0.1))), 0.0075*A29)</f>
+        <v>0.107625</v>
       </c>
       <c r="D29" s="2">
-        <v>11.54</v>
+        <v>9.67</v>
       </c>
       <c r="E29">
         <v>20</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
-        <v>2.8849999999999997E-2</v>
-      </c>
-      <c r="G29" s="1">
+        <f>MAX(IF(E29=2, 0.001, IF(E29=20, 0.01, IF(E29=200, 0.1))), 0.0025*D29)</f>
+        <v>2.4175000000000002E-2</v>
+      </c>
+      <c r="G29" s="8">
         <f t="shared" si="4"/>
-        <v>29.896013864818027</v>
-      </c>
+        <v>673.86759581881529</v>
+      </c>
+      <c r="H29" s="5"/>
       <c r="I29" t="s">
         <v>29</v>
       </c>
       <c r="J29">
-        <v>33.4</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="K29">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="P29" s="2">
         <v>0.40100000000000002</v>
@@ -1603,31 +1642,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>0.40100000000000002</v>
+        <v>16.89</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" si="1"/>
-        <v>3.0075000000000002E-3</v>
+        <f>MAX(IF(B30=2, 0.001, IF(B30=20, 0.01, IF(B30=200, 0.1))), 0.0075*A30)</f>
+        <v>0.12667500000000001</v>
       </c>
       <c r="D30" s="2">
-        <v>13.41</v>
+        <v>11.38</v>
       </c>
       <c r="E30">
         <v>20</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
-        <v>3.3524999999999999E-2</v>
-      </c>
-      <c r="G30" s="1">
+        <f>MAX(IF(E30=2, 0.001, IF(E30=20, 0.01, IF(E30=200, 0.1))), 0.0025*D30)</f>
+        <v>2.8450000000000003E-2</v>
+      </c>
+      <c r="G30" s="8">
         <f t="shared" si="4"/>
-        <v>29.903057419835942</v>
-      </c>
+        <v>673.7714624037892</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" t="s">
         <v>28</v>
       </c>
@@ -1635,10 +1675,10 @@
         <v>30</v>
       </c>
       <c r="K30">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="L30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P30" s="2">
         <v>0.45600000000000002</v>
@@ -1650,42 +1690,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>0.45600000000000002</v>
+        <v>18.55</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" si="1"/>
-        <v>3.4199999999999999E-3</v>
+        <f>MAX(IF(B31=2, 0.001, IF(B31=20, 0.01, IF(B31=200, 0.1))), 0.0075*A31)</f>
+        <v>0.139125</v>
       </c>
       <c r="D31" s="2">
-        <v>15.23</v>
+        <v>12.45</v>
       </c>
       <c r="E31">
         <v>20</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>3.8075000000000005E-2</v>
-      </c>
-      <c r="G31" s="1">
+        <f>MAX(IF(E31=2, 0.001, IF(E31=20, 0.01, IF(E31=200, 0.1))), 0.0025*D31)</f>
+        <v>3.1125E-2</v>
+      </c>
+      <c r="G31" s="8">
         <f t="shared" si="4"/>
-        <v>29.940906106369006</v>
-      </c>
+        <v>671.1590296495956</v>
+      </c>
+      <c r="H31" s="5"/>
       <c r="I31" t="s">
         <v>27</v>
       </c>
       <c r="J31">
-        <v>33.4</v>
+        <f>J29*1000</f>
+        <v>675</v>
       </c>
       <c r="K31">
-        <v>33</v>
+        <f>K29*K30</f>
+        <v>680</v>
       </c>
       <c r="L31" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="P31" s="2">
         <v>0.51800000000000002</v>
@@ -1697,41 +1740,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>0.51800000000000002</v>
+        <v>23.8</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="1"/>
-        <v>3.885E-3</v>
+        <f>MAX(IF(B32=2, 0.001, IF(B32=20, 0.01, IF(B32=200, 0.1))), 0.0075*A32)</f>
+        <v>0.17849999999999999</v>
       </c>
       <c r="D32" s="2">
-        <v>17.37</v>
+        <v>15.97</v>
       </c>
       <c r="E32">
         <v>20</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>4.3425000000000005E-2</v>
-      </c>
-      <c r="G32" s="1">
+        <f>MAX(IF(E32=2, 0.001, IF(E32=20, 0.01, IF(E32=200, 0.1))), 0.0025*D32)</f>
+        <v>3.9925000000000002E-2</v>
+      </c>
+      <c r="G32" s="8">
         <f t="shared" si="4"/>
-        <v>29.821531375935518</v>
-      </c>
+        <v>671.00840336134456</v>
+      </c>
+      <c r="H32" s="5"/>
       <c r="I32" t="s">
         <v>26</v>
       </c>
       <c r="J32">
-        <f>MAX(0.1*1,IF(J30=200,0.005*J31,0.002*J31))</f>
-        <v>0.1</v>
+        <f>MAX(0.001*1000,IF(J30=200,0.005*J31,0.002*J31))</f>
+        <v>1.35</v>
       </c>
       <c r="K32">
         <f>0.05*K31</f>
-        <v>1.6500000000000001</v>
+        <v>34</v>
       </c>
       <c r="L32" t="s">
         <v>23</v>
@@ -1748,29 +1792,30 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>0.58499999999999996</v>
+        <v>26.2</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" si="1"/>
-        <v>4.3874999999999999E-3</v>
-      </c>
-      <c r="D33" s="2">
-        <v>19.55</v>
+        <f>MAX(IF(B33=2, 0.001, IF(B33=20, 0.01, IF(B33=200, 0.1))), 0.0075*A33)</f>
+        <v>0.19649999999999998</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E33">
         <v>20</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
-        <v>4.8875000000000002E-2</v>
-      </c>
-      <c r="G33" s="1">
+        <f>MAX(IF(E33=2, 0.001, IF(E33=20, 0.01, IF(E33=200, 0.1))), 0.0025*D33)</f>
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="G33" s="8">
         <f t="shared" si="4"/>
-        <v>29.923273657289002</v>
-      </c>
+        <v>667.93893129771004</v>
+      </c>
+      <c r="H33" s="5"/>
       <c r="P33" s="2">
         <v>1.96</v>
       </c>
@@ -1782,10 +1827,6 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="2"/>
-      <c r="G34" s="1"/>
       <c r="P34" s="2">
         <v>7.34</v>
       </c>
@@ -1798,29 +1839,30 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>1.96</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" si="1"/>
-        <v>1.47E-2</v>
+        <f t="shared" ref="C35:C44" si="5">MAX(IF(B35=2, 0.001, IF(B35=20, 0.01, IF(B35=200, 0.1))), 0.0075*A35)</f>
+        <v>3.885E-3</v>
       </c>
       <c r="D35" s="2">
-        <v>1.33</v>
+        <v>4.34</v>
       </c>
       <c r="E35">
         <v>20</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
-        <v>0.01</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" ref="G35:G44" si="5">A35*1000/D35</f>
-        <v>1473.6842105263156</v>
-      </c>
+        <f t="shared" ref="F35:F44" si="6">MAX(IF(E35=2, 0.001, IF(E35=20, 0.01, IF(E35=200, 0.1))), 0.0025*D35)</f>
+        <v>1.085E-2</v>
+      </c>
+      <c r="G35" s="8">
+        <f t="shared" si="4"/>
+        <v>8378.3783783783783</v>
+      </c>
+      <c r="H35"/>
       <c r="P35" s="2">
         <v>8.2200000000000006</v>
       </c>
@@ -1833,29 +1875,30 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>7.34</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C36" s="4">
-        <f t="shared" si="1"/>
-        <v>5.5049999999999995E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.0625000000000002E-3</v>
       </c>
       <c r="D36" s="2">
-        <v>4.96</v>
+        <v>5.58</v>
       </c>
       <c r="E36">
         <v>20</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
-        <v>1.24E-2</v>
-      </c>
-      <c r="G36" s="1">
-        <f t="shared" si="5"/>
-        <v>1479.8387096774193</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>1.3950000000000001E-2</v>
+      </c>
+      <c r="G36" s="8">
+        <f t="shared" si="4"/>
+        <v>8266.6666666666661</v>
+      </c>
+      <c r="H36"/>
       <c r="I36" t="s">
         <v>15</v>
       </c>
@@ -1877,40 +1920,41 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>8.2200000000000006</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C37" s="4">
-        <f t="shared" si="1"/>
-        <v>6.1650000000000003E-2</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>5.8875000000000004E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>6.49</v>
       </c>
       <c r="E37">
         <v>20</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
-        <v>1.375E-2</v>
-      </c>
-      <c r="G37" s="1">
-        <f t="shared" si="5"/>
-        <v>1494.5454545454545</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>1.6225E-2</v>
+      </c>
+      <c r="G37" s="8">
+        <f t="shared" si="4"/>
+        <v>8267.5159235668798</v>
+      </c>
+      <c r="H37" s="3"/>
       <c r="I37">
         <f>AVERAGE(G35:G44)</f>
-        <v>1485.7008493671981</v>
+        <v>8280.1405173693984</v>
       </c>
       <c r="J37">
         <f>STDEV(G35:G44)</f>
-        <v>7.1855196018951366</v>
+        <v>35.028808208315425</v>
       </c>
       <c r="K37">
         <f>J37/COUNT(G35:G44)</f>
-        <v>0.71855196018951362</v>
+        <v>3.5028808208315425</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>7</v>
@@ -1924,29 +1968,30 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>10.77</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C38" s="4">
-        <f t="shared" si="1"/>
-        <v>8.0775E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.9449999999999998E-3</v>
       </c>
       <c r="D38" s="2">
-        <v>7.27</v>
+        <v>7.65</v>
       </c>
       <c r="E38">
         <v>20</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
-        <v>1.8175E-2</v>
-      </c>
-      <c r="G38" s="1">
-        <f t="shared" si="5"/>
-        <v>1481.4305364511692</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>1.9125E-2</v>
+      </c>
+      <c r="G38" s="8">
+        <f t="shared" si="4"/>
+        <v>8261.3390928725694</v>
+      </c>
+      <c r="H38"/>
       <c r="P38" s="2">
         <v>14.35</v>
       </c>
@@ -1959,29 +2004,30 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" si="1"/>
-        <v>8.6249999999999993E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.9500000000000005E-3</v>
       </c>
       <c r="D39" s="2">
-        <v>7.76</v>
+        <v>8.77</v>
       </c>
       <c r="E39">
         <v>20</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
-        <v>1.9400000000000001E-2</v>
-      </c>
-      <c r="G39" s="1">
-        <f t="shared" si="5"/>
-        <v>1481.9587628865979</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>2.1925E-2</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="4"/>
+        <v>8273.5849056603765</v>
+      </c>
+      <c r="H39"/>
       <c r="J39" t="s">
         <v>18</v>
       </c>
@@ -2000,40 +2046,41 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>14.35</v>
+        <v>1.3819999999999999</v>
       </c>
       <c r="B40">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C40" s="4">
-        <f t="shared" si="1"/>
-        <v>0.107625</v>
+        <f t="shared" si="5"/>
+        <v>1.0364999999999999E-2</v>
       </c>
       <c r="D40" s="2">
-        <v>9.67</v>
+        <v>11.43</v>
       </c>
       <c r="E40">
         <v>20</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
-        <v>2.4175000000000002E-2</v>
-      </c>
-      <c r="G40" s="1">
-        <f t="shared" si="5"/>
-        <v>1483.9710444674251</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>2.8575E-2</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="4"/>
+        <v>8270.6222865412437</v>
+      </c>
+      <c r="H40"/>
       <c r="I40" t="s">
         <v>29</v>
       </c>
       <c r="J40">
-        <v>0.67500000000000004</v>
+        <v>8.27</v>
       </c>
       <c r="K40">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="L40" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="P40" s="2">
         <v>18.55</v>
@@ -2047,40 +2094,41 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>16.89</v>
+        <v>1.448</v>
       </c>
       <c r="B41">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12667500000000001</v>
+        <f t="shared" si="5"/>
+        <v>1.086E-2</v>
       </c>
       <c r="D41" s="2">
-        <v>11.38</v>
+        <v>11.97</v>
       </c>
       <c r="E41">
         <v>20</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
-        <v>2.8450000000000003E-2</v>
-      </c>
-      <c r="G41" s="1">
-        <f t="shared" si="5"/>
-        <v>1484.1827768014059</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>2.9925000000000004E-2</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="4"/>
+        <v>8266.5745856353606</v>
+      </c>
+      <c r="H41"/>
       <c r="I41" t="s">
         <v>28</v>
       </c>
-      <c r="J41" t="s">
-        <v>31</v>
+      <c r="J41">
+        <v>20</v>
       </c>
       <c r="K41">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="L41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P41" s="2">
         <v>23.8</v>
@@ -2094,42 +2142,43 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>18.55</v>
+        <v>1.6659999999999999</v>
       </c>
       <c r="B42">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" si="1"/>
-        <v>0.139125</v>
+        <f t="shared" si="5"/>
+        <v>1.2494999999999999E-2</v>
       </c>
       <c r="D42" s="2">
-        <v>12.45</v>
+        <v>13.78</v>
       </c>
       <c r="E42">
         <v>20</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
-        <v>3.1125E-2</v>
-      </c>
-      <c r="G42" s="1">
-        <f t="shared" si="5"/>
-        <v>1489.9598393574297</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>3.4450000000000001E-2</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="4"/>
+        <v>8271.3085234093633</v>
+      </c>
+      <c r="H42"/>
       <c r="I42" t="s">
         <v>27</v>
       </c>
       <c r="J42">
         <f>J40*1000</f>
-        <v>675</v>
+        <v>8270</v>
       </c>
       <c r="K42">
         <f>K40*K41</f>
-        <v>680</v>
+        <v>8300</v>
       </c>
       <c r="L42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P42" s="2">
         <v>26.2</v>
@@ -2143,39 +2192,40 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>23.8</v>
+        <v>1.869</v>
       </c>
       <c r="B43">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="1"/>
-        <v>0.17849999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.4017499999999999E-2</v>
       </c>
       <c r="D43" s="2">
-        <v>15.97</v>
+        <v>15.48</v>
       </c>
       <c r="E43">
         <v>20</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
-        <v>3.9925000000000002E-2</v>
-      </c>
-      <c r="G43" s="1">
-        <f t="shared" si="5"/>
-        <v>1490.2943018159049</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>3.8700000000000005E-2</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="4"/>
+        <v>8282.504012841091</v>
+      </c>
+      <c r="H43"/>
       <c r="I43" t="s">
         <v>26</v>
       </c>
       <c r="J43">
-        <f>MAX(0.001*1000,IF(J41=200,0.005*J42,0.002*J42))</f>
-        <v>1.35</v>
+        <f>MAX(0.01*1000,IF(J41=200,0.005*J42,0.002*J42))</f>
+        <v>16.54</v>
       </c>
       <c r="K43">
         <f>0.05*K42</f>
-        <v>34</v>
+        <v>415</v>
       </c>
       <c r="L43" t="s">
         <v>23</v>
@@ -2183,38 +2233,40 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>26.2</v>
+        <v>2.13</v>
       </c>
       <c r="B44">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="1"/>
-        <v>0.19649999999999998</v>
+        <f t="shared" si="5"/>
+        <v>1.5975E-2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E44">
         <v>20</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
-        <v>4.3750000000000004E-2</v>
-      </c>
-      <c r="G44" s="1">
-        <f t="shared" si="5"/>
-        <v>1497.1428571428571</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="4"/>
+        <v>8262.9107981220659</v>
+      </c>
+      <c r="H44"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G45" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:C44">
-    <sortCondition ref="A35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A24:C33">
+    <sortCondition ref="A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ohms law lab edits
</commit_message>
<xml_diff>
--- a/ohm/PHY224 Ohm Lab.xlsx
+++ b/ohm/PHY224 Ohm Lab.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/js/school/phy224/ohm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B4FFEF-194C-F34E-8AED-1D0873BBF9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE82F9FC-5379-6745-B498-19D3D942DC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
+    <workbookView xWindow="11480" yWindow="6840" windowWidth="28800" windowHeight="17540" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>I (mA)</t>
   </si>
@@ -136,10 +137,10 @@
     <t>voltage</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
     <t>200 kOhms</t>
+  </si>
+  <si>
+    <t>orange</t>
   </si>
 </sst>
 </file>
@@ -517,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1FA504-BF5F-6343-8346-DC2B6EE3C439}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="4">
-        <f>MAX(IF(B13=2, 0.001, IF(B13=20, 0.01, IF(B13=200, 0.1))), 0.0075*A13)</f>
+        <f t="shared" ref="C13:C22" si="4">MAX(IF(B13=2, 0.001, IF(B13=20, 0.01, IF(B13=200, 0.1))), 0.0075*A13)</f>
         <v>1E-3</v>
       </c>
       <c r="D13" s="2">
@@ -1023,7 +1024,7 @@
         <v>20</v>
       </c>
       <c r="F13">
-        <f>MAX(IF(E13=2, 0.001, IF(E13=20, 0.01, IF(E13=200, 0.1))), 0.0025*D13)</f>
+        <f t="shared" ref="F13:F22" si="5">MAX(IF(E13=2, 0.001, IF(E13=20, 0.01, IF(E13=200, 0.1))), 0.0025*D13)</f>
         <v>1.1050000000000001E-2</v>
       </c>
       <c r="G13" s="8">
@@ -1031,8 +1032,15 @@
         <v>33740.45801526717</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="P13" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1042,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="4">
-        <f>MAX(IF(B14=2, 0.001, IF(B14=20, 0.01, IF(B14=200, 0.1))), 0.0075*A14)</f>
+        <f t="shared" si="4"/>
         <v>1.2750000000000001E-3</v>
       </c>
       <c r="D14" s="2">
@@ -1052,7 +1060,7 @@
         <v>20</v>
       </c>
       <c r="F14">
-        <f>MAX(IF(E14=2, 0.001, IF(E14=20, 0.01, IF(E14=200, 0.1))), 0.0025*D14)</f>
+        <f t="shared" si="5"/>
         <v>1.3925000000000002E-2</v>
       </c>
       <c r="G14" s="8">
@@ -1069,8 +1077,15 @@
       <c r="K14" t="s">
         <v>17</v>
       </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="P14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>5.57</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1080,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4">
-        <f>MAX(IF(B15=2, 0.001, IF(B15=20, 0.01, IF(B15=200, 0.1))), 0.0075*A15)</f>
+        <f t="shared" si="4"/>
         <v>1.4024999999999999E-3</v>
       </c>
       <c r="D15" s="2">
@@ -1090,7 +1105,7 @@
         <v>20</v>
       </c>
       <c r="F15">
-        <f>MAX(IF(E15=2, 0.001, IF(E15=20, 0.01, IF(E15=200, 0.1))), 0.0025*D15)</f>
+        <f t="shared" si="5"/>
         <v>1.5575000000000002E-2</v>
       </c>
       <c r="G15" s="8">
@@ -1110,8 +1125,15 @@
         <f>J15/COUNT(G13:G22)</f>
         <v>24.683250186969232</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="P15" s="2">
+        <v>0.187</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1121,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="4">
-        <f>MAX(IF(B16=2, 0.001, IF(B16=20, 0.01, IF(B16=200, 0.1))), 0.0075*A16)</f>
+        <f t="shared" si="4"/>
         <v>1.74E-3</v>
       </c>
       <c r="D16" s="2">
@@ -1131,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="F16">
-        <f>MAX(IF(E16=2, 0.001, IF(E16=20, 0.01, IF(E16=200, 0.1))), 0.0025*D16)</f>
+        <f t="shared" si="5"/>
         <v>1.9350000000000003E-2</v>
       </c>
       <c r="G16" s="8">
@@ -1139,8 +1161,15 @@
         <v>33362.068965517239</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
+      <c r="P16" s="2">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>7.74</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1150,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="4">
-        <f>MAX(IF(B17=2, 0.001, IF(B17=20, 0.01, IF(B17=200, 0.1))), 0.0075*A17)</f>
+        <f t="shared" si="4"/>
         <v>2.2575E-3</v>
       </c>
       <c r="D17" s="2">
@@ -1160,7 +1189,7 @@
         <v>20</v>
       </c>
       <c r="F17">
-        <f>MAX(IF(E17=2, 0.001, IF(E17=20, 0.01, IF(E17=200, 0.1))), 0.0025*D17)</f>
+        <f t="shared" si="5"/>
         <v>2.5150000000000002E-2</v>
       </c>
       <c r="G17" s="8">
@@ -1174,8 +1203,15 @@
       <c r="K17" t="s">
         <v>19</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
+      <c r="P17" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>10.06</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -1185,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="4">
-        <f>MAX(IF(B18=2, 0.001, IF(B18=20, 0.01, IF(B18=200, 0.1))), 0.0075*A18)</f>
+        <f t="shared" si="4"/>
         <v>2.5874999999999995E-3</v>
       </c>
       <c r="D18" s="2">
@@ -1195,7 +1231,7 @@
         <v>20</v>
       </c>
       <c r="F18">
-        <f>MAX(IF(E18=2, 0.001, IF(E18=20, 0.01, IF(E18=200, 0.1))), 0.0025*D18)</f>
+        <f t="shared" si="5"/>
         <v>2.8849999999999997E-2</v>
       </c>
       <c r="G18" s="8">
@@ -1215,8 +1251,15 @@
       <c r="L18" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="P18" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>11.54</v>
+      </c>
+      <c r="R18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -1226,7 +1269,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="4">
-        <f>MAX(IF(B19=2, 0.001, IF(B19=20, 0.01, IF(B19=200, 0.1))), 0.0075*A19)</f>
+        <f t="shared" si="4"/>
         <v>3.0075000000000002E-3</v>
       </c>
       <c r="D19" s="2">
@@ -1236,7 +1279,7 @@
         <v>20</v>
       </c>
       <c r="F19">
-        <f>MAX(IF(E19=2, 0.001, IF(E19=20, 0.01, IF(E19=200, 0.1))), 0.0025*D19)</f>
+        <f t="shared" si="5"/>
         <v>3.3524999999999999E-2</v>
       </c>
       <c r="G19" s="8">
@@ -1248,7 +1291,7 @@
         <v>28</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19">
         <v>1000</v>
@@ -1256,8 +1299,15 @@
       <c r="L19" t="s">
         <v>21</v>
       </c>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
+      <c r="P19" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>13.41</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1267,7 +1317,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="4">
-        <f>MAX(IF(B20=2, 0.001, IF(B20=20, 0.01, IF(B20=200, 0.1))), 0.0075*A20)</f>
+        <f t="shared" si="4"/>
         <v>3.4199999999999999E-3</v>
       </c>
       <c r="D20" s="2">
@@ -1277,7 +1327,7 @@
         <v>20</v>
       </c>
       <c r="F20">
-        <f>MAX(IF(E20=2, 0.001, IF(E20=20, 0.01, IF(E20=200, 0.1))), 0.0025*D20)</f>
+        <f t="shared" si="5"/>
         <v>3.8075000000000005E-2</v>
       </c>
       <c r="G20" s="8">
@@ -1295,10 +1345,17 @@
         <v>33000</v>
       </c>
       <c r="L20" t="s">
-        <v>34</v>
-      </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>15.23</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1308,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="4">
-        <f>MAX(IF(B21=2, 0.001, IF(B21=20, 0.01, IF(B21=200, 0.1))), 0.0075*A21)</f>
+        <f t="shared" si="4"/>
         <v>3.885E-3</v>
       </c>
       <c r="D21" s="2">
@@ -1318,7 +1375,7 @@
         <v>20</v>
       </c>
       <c r="F21">
-        <f>MAX(IF(E21=2, 0.001, IF(E21=20, 0.01, IF(E21=200, 0.1))), 0.0025*D21)</f>
+        <f t="shared" si="5"/>
         <v>4.3425000000000005E-2</v>
       </c>
       <c r="G21" s="8">
@@ -1340,8 +1397,15 @@
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
+      <c r="P21" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>17.37</v>
+      </c>
+      <c r="R21">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -1351,7 +1415,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="4">
-        <f>MAX(IF(B22=2, 0.001, IF(B22=20, 0.01, IF(B22=200, 0.1))), 0.0075*A22)</f>
+        <f t="shared" si="4"/>
         <v>4.3874999999999999E-3</v>
       </c>
       <c r="D22" s="2">
@@ -1361,7 +1425,7 @@
         <v>20</v>
       </c>
       <c r="F22">
-        <f>MAX(IF(E22=2, 0.001, IF(E22=20, 0.01, IF(E22=200, 0.1))), 0.0025*D22)</f>
+        <f t="shared" si="5"/>
         <v>4.8875000000000002E-2</v>
       </c>
       <c r="G22" s="8">
@@ -1369,8 +1433,15 @@
         <v>33418.803418803422</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>19.55</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
@@ -1378,10 +1449,10 @@
       <c r="D23" s="2"/>
       <c r="G23" s="1"/>
       <c r="P23" s="2">
-        <v>0.13100000000000001</v>
+        <v>1.96</v>
       </c>
       <c r="Q23" s="2">
-        <v>4.42</v>
+        <v>1.33</v>
       </c>
       <c r="R23">
         <v>3</v>
@@ -1395,7 +1466,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="4">
-        <f>MAX(IF(B24=2, 0.001, IF(B24=20, 0.01, IF(B24=200, 0.1))), 0.0075*A24)</f>
+        <f t="shared" ref="C24:C33" si="6">MAX(IF(B24=2, 0.001, IF(B24=20, 0.01, IF(B24=200, 0.1))), 0.0075*A24)</f>
         <v>1.47E-2</v>
       </c>
       <c r="D24" s="2">
@@ -1405,7 +1476,7 @@
         <v>20</v>
       </c>
       <c r="F24">
-        <f>MAX(IF(E24=2, 0.001, IF(E24=20, 0.01, IF(E24=200, 0.1))), 0.0025*D24)</f>
+        <f t="shared" ref="F24:F33" si="7">MAX(IF(E24=2, 0.001, IF(E24=20, 0.01, IF(E24=200, 0.1))), 0.0025*D24)</f>
         <v>0.01</v>
       </c>
       <c r="G24" s="8">
@@ -1413,11 +1484,11 @@
         <v>678.57142857142867</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="P24" s="2" t="s">
-        <v>6</v>
+      <c r="P24" s="2">
+        <v>7.34</v>
       </c>
       <c r="Q24" s="2">
-        <v>5.57</v>
+        <v>4.96</v>
       </c>
       <c r="R24">
         <v>3</v>
@@ -1431,7 +1502,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="4">
-        <f>MAX(IF(B25=2, 0.001, IF(B25=20, 0.01, IF(B25=200, 0.1))), 0.0075*A25)</f>
+        <f t="shared" si="6"/>
         <v>5.5049999999999995E-2</v>
       </c>
       <c r="D25" s="2">
@@ -1441,11 +1512,11 @@
         <v>20</v>
       </c>
       <c r="F25">
-        <f>MAX(IF(E25=2, 0.001, IF(E25=20, 0.01, IF(E25=200, 0.1))), 0.0025*D25)</f>
+        <f t="shared" si="7"/>
         <v>1.24E-2</v>
       </c>
       <c r="G25" s="8">
-        <f t="shared" ref="G25:G44" si="4">D25/(A25/1000)</f>
+        <f t="shared" ref="G25:G44" si="8">D25/(A25/1000)</f>
         <v>675.74931880108988</v>
       </c>
       <c r="H25" s="5"/>
@@ -1459,10 +1530,10 @@
         <v>17</v>
       </c>
       <c r="P25" s="2">
-        <v>0.187</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>6.23</v>
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="R25">
         <v>3</v>
@@ -1476,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="4">
-        <f>MAX(IF(B26=2, 0.001, IF(B26=20, 0.01, IF(B26=200, 0.1))), 0.0075*A26)</f>
+        <f t="shared" si="6"/>
         <v>6.1650000000000003E-2</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1486,11 +1557,11 @@
         <v>20</v>
       </c>
       <c r="F26">
-        <f>MAX(IF(E26=2, 0.001, IF(E26=20, 0.01, IF(E26=200, 0.1))), 0.0025*D26)</f>
+        <f t="shared" si="7"/>
         <v>1.375E-2</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>669.09975669099754</v>
       </c>
       <c r="H26" s="5"/>
@@ -1507,10 +1578,10 @@
         <v>0.32541604809105024</v>
       </c>
       <c r="P26" s="2">
-        <v>0.23200000000000001</v>
+        <v>10.77</v>
       </c>
       <c r="Q26" s="2">
-        <v>7.74</v>
+        <v>7.27</v>
       </c>
       <c r="R26">
         <v>3</v>
@@ -1524,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="4">
-        <f>MAX(IF(B27=2, 0.001, IF(B27=20, 0.01, IF(B27=200, 0.1))), 0.0075*A27)</f>
+        <f t="shared" si="6"/>
         <v>8.0775E-2</v>
       </c>
       <c r="D27" s="2">
@@ -1534,19 +1605,19 @@
         <v>20</v>
       </c>
       <c r="F27">
-        <f>MAX(IF(E27=2, 0.001, IF(E27=20, 0.01, IF(E27=200, 0.1))), 0.0025*D27)</f>
+        <f t="shared" si="7"/>
         <v>1.8175E-2</v>
       </c>
       <c r="G27" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>675.02321262766941</v>
       </c>
       <c r="H27" s="5"/>
-      <c r="P27" s="2">
-        <v>0.30099999999999999</v>
+      <c r="P27" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="Q27" s="2">
-        <v>10.06</v>
+        <v>7.76</v>
       </c>
       <c r="R27">
         <v>3</v>
@@ -1560,7 +1631,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="4">
-        <f>MAX(IF(B28=2, 0.001, IF(B28=20, 0.01, IF(B28=200, 0.1))), 0.0075*A28)</f>
+        <f t="shared" si="6"/>
         <v>8.6249999999999993E-2</v>
       </c>
       <c r="D28" s="2">
@@ -1570,11 +1641,11 @@
         <v>20</v>
       </c>
       <c r="F28">
-        <f>MAX(IF(E28=2, 0.001, IF(E28=20, 0.01, IF(E28=200, 0.1))), 0.0025*D28)</f>
+        <f t="shared" si="7"/>
         <v>1.9400000000000001E-2</v>
       </c>
       <c r="G28" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>674.78260869565213</v>
       </c>
       <c r="H28" s="5"/>
@@ -1585,10 +1656,10 @@
         <v>19</v>
       </c>
       <c r="P28" s="2">
-        <v>0.34499999999999997</v>
+        <v>14.35</v>
       </c>
       <c r="Q28" s="2">
-        <v>11.54</v>
+        <v>9.67</v>
       </c>
       <c r="R28">
         <v>3</v>
@@ -1602,7 +1673,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="4">
-        <f>MAX(IF(B29=2, 0.001, IF(B29=20, 0.01, IF(B29=200, 0.1))), 0.0075*A29)</f>
+        <f t="shared" si="6"/>
         <v>0.107625</v>
       </c>
       <c r="D29" s="2">
@@ -1612,11 +1683,11 @@
         <v>20</v>
       </c>
       <c r="F29">
-        <f>MAX(IF(E29=2, 0.001, IF(E29=20, 0.01, IF(E29=200, 0.1))), 0.0025*D29)</f>
+        <f t="shared" si="7"/>
         <v>2.4175000000000002E-2</v>
       </c>
       <c r="G29" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>673.86759581881529</v>
       </c>
       <c r="H29" s="5"/>
@@ -1633,10 +1704,10 @@
         <v>25</v>
       </c>
       <c r="P29" s="2">
-        <v>0.40100000000000002</v>
+        <v>16.89</v>
       </c>
       <c r="Q29" s="2">
-        <v>13.41</v>
+        <v>11.38</v>
       </c>
       <c r="R29">
         <v>3</v>
@@ -1650,7 +1721,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="4">
-        <f>MAX(IF(B30=2, 0.001, IF(B30=20, 0.01, IF(B30=200, 0.1))), 0.0075*A30)</f>
+        <f t="shared" si="6"/>
         <v>0.12667500000000001</v>
       </c>
       <c r="D30" s="2">
@@ -1660,11 +1731,11 @@
         <v>20</v>
       </c>
       <c r="F30">
-        <f>MAX(IF(E30=2, 0.001, IF(E30=20, 0.01, IF(E30=200, 0.1))), 0.0025*D30)</f>
+        <f t="shared" si="7"/>
         <v>2.8450000000000003E-2</v>
       </c>
       <c r="G30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>673.7714624037892</v>
       </c>
       <c r="H30" s="5"/>
@@ -1681,10 +1752,10 @@
         <v>20</v>
       </c>
       <c r="P30" s="2">
-        <v>0.45600000000000002</v>
+        <v>18.55</v>
       </c>
       <c r="Q30" s="2">
-        <v>15.23</v>
+        <v>12.45</v>
       </c>
       <c r="R30">
         <v>3</v>
@@ -1698,7 +1769,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="4">
-        <f>MAX(IF(B31=2, 0.001, IF(B31=20, 0.01, IF(B31=200, 0.1))), 0.0075*A31)</f>
+        <f t="shared" si="6"/>
         <v>0.139125</v>
       </c>
       <c r="D31" s="2">
@@ -1708,11 +1779,11 @@
         <v>20</v>
       </c>
       <c r="F31">
-        <f>MAX(IF(E31=2, 0.001, IF(E31=20, 0.01, IF(E31=200, 0.1))), 0.0025*D31)</f>
+        <f t="shared" si="7"/>
         <v>3.1125E-2</v>
       </c>
       <c r="G31" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>671.1590296495956</v>
       </c>
       <c r="H31" s="5"/>
@@ -1731,10 +1802,10 @@
         <v>22</v>
       </c>
       <c r="P31" s="2">
-        <v>0.51800000000000002</v>
+        <v>23.8</v>
       </c>
       <c r="Q31" s="2">
-        <v>17.37</v>
+        <v>15.97</v>
       </c>
       <c r="R31">
         <v>3</v>
@@ -1748,7 +1819,7 @@
         <v>200</v>
       </c>
       <c r="C32" s="4">
-        <f>MAX(IF(B32=2, 0.001, IF(B32=20, 0.01, IF(B32=200, 0.1))), 0.0075*A32)</f>
+        <f t="shared" si="6"/>
         <v>0.17849999999999999</v>
       </c>
       <c r="D32" s="2">
@@ -1758,11 +1829,11 @@
         <v>20</v>
       </c>
       <c r="F32">
-        <f>MAX(IF(E32=2, 0.001, IF(E32=20, 0.01, IF(E32=200, 0.1))), 0.0025*D32)</f>
+        <f t="shared" si="7"/>
         <v>3.9925000000000002E-2</v>
       </c>
       <c r="G32" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>671.00840336134456</v>
       </c>
       <c r="H32" s="5"/>
@@ -1781,10 +1852,10 @@
         <v>23</v>
       </c>
       <c r="P32" s="2">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>19.55</v>
+        <v>26.2</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="R32">
         <v>3</v>
@@ -1798,7 +1869,7 @@
         <v>200</v>
       </c>
       <c r="C33" s="4">
-        <f>MAX(IF(B33=2, 0.001, IF(B33=20, 0.01, IF(B33=200, 0.1))), 0.0075*A33)</f>
+        <f t="shared" si="6"/>
         <v>0.19649999999999998</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1808,19 +1879,19 @@
         <v>20</v>
       </c>
       <c r="F33">
-        <f>MAX(IF(E33=2, 0.001, IF(E33=20, 0.01, IF(E33=200, 0.1))), 0.0025*D33)</f>
+        <f t="shared" si="7"/>
         <v>4.3750000000000004E-2</v>
       </c>
       <c r="G33" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>667.93893129771004</v>
       </c>
       <c r="H33" s="5"/>
       <c r="P33" s="2">
-        <v>1.96</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="Q33" s="2">
-        <v>1.33</v>
+        <v>4.34</v>
       </c>
       <c r="R33">
         <v>4</v>
@@ -1828,10 +1899,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P34" s="2">
-        <v>7.34</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="Q34" s="2">
-        <v>4.96</v>
+        <v>5.58</v>
       </c>
       <c r="R34">
         <v>4</v>
@@ -1845,7 +1916,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" ref="C35:C44" si="5">MAX(IF(B35=2, 0.001, IF(B35=20, 0.01, IF(B35=200, 0.1))), 0.0075*A35)</f>
+        <f t="shared" ref="C35:C44" si="9">MAX(IF(B35=2, 0.001, IF(B35=20, 0.01, IF(B35=200, 0.1))), 0.0075*A35)</f>
         <v>3.885E-3</v>
       </c>
       <c r="D35" s="2">
@@ -1855,19 +1926,19 @@
         <v>20</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F44" si="6">MAX(IF(E35=2, 0.001, IF(E35=20, 0.01, IF(E35=200, 0.1))), 0.0025*D35)</f>
+        <f t="shared" ref="F35:F44" si="10">MAX(IF(E35=2, 0.001, IF(E35=20, 0.01, IF(E35=200, 0.1))), 0.0025*D35)</f>
         <v>1.085E-2</v>
       </c>
       <c r="G35" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8378.3783783783783</v>
       </c>
       <c r="H35"/>
       <c r="P35" s="2">
-        <v>8.2200000000000006</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>8</v>
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>6.49</v>
       </c>
       <c r="R35">
         <v>4</v>
@@ -1881,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5.0625000000000002E-3</v>
       </c>
       <c r="D36" s="2">
@@ -1891,11 +1962,11 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.3950000000000001E-2</v>
       </c>
       <c r="G36" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8266.6666666666661</v>
       </c>
       <c r="H36"/>
@@ -1909,10 +1980,10 @@
         <v>17</v>
       </c>
       <c r="P36" s="2">
-        <v>10.77</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="Q36" s="2">
-        <v>7.27</v>
+        <v>7.65</v>
       </c>
       <c r="R36">
         <v>4</v>
@@ -1926,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5.8875000000000004E-3</v>
       </c>
       <c r="D37" s="2">
@@ -1936,11 +2007,11 @@
         <v>20</v>
       </c>
       <c r="F37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.6225E-2</v>
       </c>
       <c r="G37" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8267.5159235668798</v>
       </c>
       <c r="H37" s="3"/>
@@ -1957,10 +2028,10 @@
         <v>3.5028808208315425</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q37" s="2">
-        <v>7.76</v>
+        <v>8.77</v>
       </c>
       <c r="R37">
         <v>4</v>
@@ -1974,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.9449999999999998E-3</v>
       </c>
       <c r="D38" s="2">
@@ -1984,19 +2055,19 @@
         <v>20</v>
       </c>
       <c r="F38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.9125E-2</v>
       </c>
       <c r="G38" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8261.3390928725694</v>
       </c>
       <c r="H38"/>
       <c r="P38" s="2">
-        <v>14.35</v>
+        <v>1.3819999999999999</v>
       </c>
       <c r="Q38" s="2">
-        <v>9.67</v>
+        <v>11.43</v>
       </c>
       <c r="R38">
         <v>4</v>
@@ -2010,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.9500000000000005E-3</v>
       </c>
       <c r="D39" s="2">
@@ -2020,11 +2091,11 @@
         <v>20</v>
       </c>
       <c r="F39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.1925E-2</v>
       </c>
       <c r="G39" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8273.5849056603765</v>
       </c>
       <c r="H39"/>
@@ -2035,10 +2106,10 @@
         <v>19</v>
       </c>
       <c r="P39" s="2">
-        <v>16.89</v>
+        <v>1.448</v>
       </c>
       <c r="Q39" s="2">
-        <v>11.38</v>
+        <v>11.97</v>
       </c>
       <c r="R39">
         <v>4</v>
@@ -2052,7 +2123,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.0364999999999999E-2</v>
       </c>
       <c r="D40" s="2">
@@ -2062,11 +2133,11 @@
         <v>20</v>
       </c>
       <c r="F40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.8575E-2</v>
       </c>
       <c r="G40" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8270.6222865412437</v>
       </c>
       <c r="H40"/>
@@ -2083,10 +2154,10 @@
         <v>20</v>
       </c>
       <c r="P40" s="2">
-        <v>18.55</v>
+        <v>1.6659999999999999</v>
       </c>
       <c r="Q40" s="2">
-        <v>12.45</v>
+        <v>13.78</v>
       </c>
       <c r="R40">
         <v>4</v>
@@ -2100,7 +2171,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.086E-2</v>
       </c>
       <c r="D41" s="2">
@@ -2110,11 +2181,11 @@
         <v>20</v>
       </c>
       <c r="F41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.9925000000000004E-2</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8266.5745856353606</v>
       </c>
       <c r="H41"/>
@@ -2131,10 +2202,10 @@
         <v>21</v>
       </c>
       <c r="P41" s="2">
-        <v>23.8</v>
+        <v>1.869</v>
       </c>
       <c r="Q41" s="2">
-        <v>15.97</v>
+        <v>15.48</v>
       </c>
       <c r="R41">
         <v>4</v>
@@ -2148,7 +2219,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.2494999999999999E-2</v>
       </c>
       <c r="D42" s="2">
@@ -2158,11 +2229,11 @@
         <v>20</v>
       </c>
       <c r="F42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.4450000000000001E-2</v>
       </c>
       <c r="G42" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8271.3085234093633</v>
       </c>
       <c r="H42"/>
@@ -2181,10 +2252,10 @@
         <v>24</v>
       </c>
       <c r="P42" s="2">
-        <v>26.2</v>
+        <v>2.13</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R42">
         <v>4</v>
@@ -2198,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.4017499999999999E-2</v>
       </c>
       <c r="D43" s="2">
@@ -2208,11 +2279,11 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.8700000000000005E-2</v>
       </c>
       <c r="G43" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8282.504012841091</v>
       </c>
       <c r="H43"/>
@@ -2239,7 +2310,7 @@
         <v>20</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.5975E-2</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2249,11 +2320,11 @@
         <v>20</v>
       </c>
       <c r="F44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.4000000000000004E-2</v>
       </c>
       <c r="G44" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8262.9107981220659</v>
       </c>
       <c r="H44"/>
@@ -2271,6 +2342,461 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7548BC-6D4C-8041-9570-DA2E9C9D80FF}">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>1.373</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>3.81</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5.12</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5.53</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>9.36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>9.49</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7.72</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>14.22</v>
+      </c>
+      <c r="B7" s="2">
+        <v>11.56</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>15.57</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12.67</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>17.07</v>
+      </c>
+      <c r="B9" s="2">
+        <v>13.83</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>19.36</v>
+      </c>
+      <c r="B10" s="2">
+        <v>15.64</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5.57</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>0.187</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7.74</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="B15" s="2">
+        <v>10.06</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11.54</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13.41</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="B18" s="2">
+        <v>15.23</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="B19" s="2">
+        <v>17.37</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19.55</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>7.34</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4.96</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>10.77</v>
+      </c>
+      <c r="B24" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.76</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>14.35</v>
+      </c>
+      <c r="B26" s="2">
+        <v>9.67</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>16.89</v>
+      </c>
+      <c r="B27" s="2">
+        <v>11.38</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>18.55</v>
+      </c>
+      <c r="B28" s="2">
+        <v>12.45</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="B29" s="2">
+        <v>15.97</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4.34</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="B32" s="2">
+        <v>5.58</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="B33" s="2">
+        <v>6.49</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="B34" s="2">
+        <v>7.65</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="2">
+        <v>8.77</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>1.3819999999999999</v>
+      </c>
+      <c r="B36" s="2">
+        <v>11.43</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>1.448</v>
+      </c>
+      <c r="B37" s="2">
+        <v>11.97</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="B38" s="2">
+        <v>13.78</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1.869</v>
+      </c>
+      <c r="B39" s="2">
+        <v>15.48</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>2.13</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9FA899-4D84-6343-BA2A-7F0ADCCB1FAD}">
   <dimension ref="A1:C40"/>
   <sheetViews>

</xml_diff>

<commit_message>
ohms law lab (pylab1) finalized
</commit_message>
<xml_diff>
--- a/ohm/PHY224 Ohm Lab.xlsx
+++ b/ohm/PHY224 Ohm Lab.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/js/school/phy224/ohm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE82F9FC-5379-6745-B498-19D3D942DC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F101F33-C553-9C41-BCE7-F8C7A691552A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="6840" windowWidth="28800" windowHeight="17540" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
+    <workbookView xWindow="16800" yWindow="2260" windowWidth="21600" windowHeight="17540" xr2:uid="{D29481CB-EE21-594F-8C6B-39684760DC86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>I (mA)</t>
   </si>
@@ -174,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,11 +188,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -199,7 +220,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -217,6 +246,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="F2">
+            <v>3.2975000000000001E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1FA504-BF5F-6343-8346-DC2B6EE3C439}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,27 +601,27 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="8">
         <v>1.373</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="9">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
         <f>MAX(IF(B2=2, 0.001, IF(B2=20, 0.01, IF(B2=200, 0.1))), 0.0075*A2)</f>
         <v>1.0297499999999999E-2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="8">
         <v>1.1220000000000001</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <f>MAX(IF(E2=2, 0.001, IF(E2=20, 0.01, IF(E2=200, 0.1))), 0.0025*D2)</f>
-        <v>2.8050000000000002E-3</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="E2" s="9">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9" t="b">
+        <f>[1]data!$F$2=MAX(IF(E2=2, 0.001, IF(E2=20, 0.01, IF(E2=200, 0.1))), 0.0025*D2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
         <f t="shared" ref="G2:G10" si="0">D2/(A2/1000)</f>
         <v>817.18863801893667</v>
       </c>
@@ -589,27 +637,27 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="8">
         <v>3.81</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="9">
+        <v>20</v>
+      </c>
+      <c r="C3" s="10">
         <f t="shared" ref="C3:C11" si="1">MAX(IF(B3=2, 0.001, IF(B3=20, 0.01, IF(B3=200, 0.1))), 0.0075*A3)</f>
         <v>2.8575E-2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>3.11</v>
       </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="9">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9">
         <f t="shared" ref="F3:F11" si="2">MAX(IF(E3=2, 0.001, IF(E3=20, 0.01, IF(E3=200, 0.1))), 0.0025*D3)</f>
         <v>0.01</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="11">
         <f t="shared" si="0"/>
         <v>816.27296587926503</v>
       </c>
@@ -634,27 +682,27 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="9">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10">
         <f t="shared" si="1"/>
         <v>4.725E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>5.12</v>
       </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="9">
+        <v>20</v>
+      </c>
+      <c r="F4" s="9">
         <f t="shared" si="2"/>
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>812.69841269841265</v>
       </c>
@@ -682,27 +730,27 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="8">
         <v>6.82</v>
       </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="9">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
         <f t="shared" si="1"/>
         <v>5.1150000000000001E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>5.53</v>
       </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="9">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9">
         <f t="shared" si="2"/>
         <v>1.3825E-2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>810.85043988269797</v>
       </c>
@@ -718,27 +766,27 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="8">
         <v>9.36</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="9">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10">
         <f t="shared" si="1"/>
         <v>7.0199999999999999E-2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="9">
+        <v>20</v>
+      </c>
+      <c r="F6" s="9">
         <f t="shared" si="2"/>
         <v>1.9E-2</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>811.96581196581189</v>
       </c>
@@ -760,27 +808,27 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="8">
         <v>9.49</v>
       </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="9">
+        <v>20</v>
+      </c>
+      <c r="C7" s="10">
         <f t="shared" si="1"/>
         <v>7.1175000000000002E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <v>7.72</v>
       </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="9">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9">
         <f t="shared" si="2"/>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>813.48788198103261</v>
       </c>
@@ -808,27 +856,27 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="8">
         <v>14.22</v>
       </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="9">
+        <v>20</v>
+      </c>
+      <c r="C8" s="10">
         <f t="shared" si="1"/>
         <v>0.10664999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="8">
         <v>11.56</v>
       </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="9">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9">
         <f t="shared" si="2"/>
         <v>2.8900000000000002E-2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>812.93952180028134</v>
       </c>
@@ -856,27 +904,27 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="8">
         <v>15.57</v>
       </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="10">
         <f t="shared" si="1"/>
         <v>0.116775</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="8">
         <v>12.67</v>
       </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="9">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9">
         <f t="shared" si="2"/>
         <v>3.1675000000000002E-2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>813.74438021836863</v>
       </c>
@@ -906,27 +954,27 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <v>17.07</v>
       </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="9">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10">
         <f t="shared" si="1"/>
         <v>0.128025</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>13.83</v>
       </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="9">
+        <v>20</v>
+      </c>
+      <c r="F10" s="9">
         <f t="shared" si="2"/>
         <v>3.4575000000000002E-2</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>810.19332161687157</v>
       </c>
@@ -956,27 +1004,27 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="8">
         <v>19.36</v>
       </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="9">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10">
         <f t="shared" si="1"/>
         <v>0.1452</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>15.64</v>
       </c>
-      <c r="E11">
-        <v>20</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="9">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9">
         <f t="shared" si="2"/>
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="11">
         <f t="shared" ref="G11:G21" si="3">D11/(A11/1000)</f>
         <v>807.8512396694216</v>
       </c>
@@ -992,10 +1040,13 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12"/>
       <c r="P12" s="2">
         <v>19.36</v>
       </c>
@@ -1007,27 +1058,27 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="8">
         <v>0.13100000000000001</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10">
         <f t="shared" ref="C13:C22" si="4">MAX(IF(B13=2, 0.001, IF(B13=20, 0.01, IF(B13=200, 0.1))), 0.0075*A13)</f>
         <v>1E-3</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <v>4.42</v>
       </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="9">
+        <v>20</v>
+      </c>
+      <c r="F13" s="9">
         <f t="shared" ref="F13:F22" si="5">MAX(IF(E13=2, 0.001, IF(E13=20, 0.01, IF(E13=200, 0.1))), 0.0025*D13)</f>
         <v>1.1050000000000001E-2</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="11">
         <f t="shared" si="3"/>
         <v>33740.45801526717</v>
       </c>
@@ -1043,27 +1094,27 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="10">
         <f t="shared" si="4"/>
         <v>1.2750000000000001E-3</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="8">
         <v>5.57</v>
       </c>
-      <c r="E14">
-        <v>20</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="9">
+        <v>20</v>
+      </c>
+      <c r="F14" s="9">
         <f t="shared" si="5"/>
         <v>1.3925000000000002E-2</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="11">
         <f t="shared" si="3"/>
         <v>32764.705882352941</v>
       </c>
@@ -1088,27 +1139,27 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="8">
         <v>0.187</v>
       </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10">
         <f t="shared" si="4"/>
         <v>1.4024999999999999E-3</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="8">
         <v>6.23</v>
       </c>
-      <c r="E15">
-        <v>20</v>
-      </c>
-      <c r="F15">
+      <c r="E15" s="9">
+        <v>20</v>
+      </c>
+      <c r="F15" s="9">
         <f t="shared" si="5"/>
         <v>1.5575000000000002E-2</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="11">
         <f t="shared" si="3"/>
         <v>33315.508021390378</v>
       </c>
@@ -1136,27 +1187,27 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="8">
         <v>0.23200000000000001</v>
       </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10">
         <f t="shared" si="4"/>
         <v>1.74E-3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <v>7.74</v>
       </c>
-      <c r="E16">
-        <v>20</v>
-      </c>
-      <c r="F16">
+      <c r="E16" s="9">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9">
         <f t="shared" si="5"/>
         <v>1.9350000000000003E-2</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="11">
         <f t="shared" si="3"/>
         <v>33362.068965517239</v>
       </c>
@@ -1172,27 +1223,27 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="8">
         <v>0.30099999999999999</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B17" s="9">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10">
         <f t="shared" si="4"/>
         <v>2.2575E-3</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="8">
         <v>10.06</v>
       </c>
-      <c r="E17">
-        <v>20</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="9">
+        <v>20</v>
+      </c>
+      <c r="F17" s="9">
         <f t="shared" si="5"/>
         <v>2.5150000000000002E-2</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="11">
         <f t="shared" si="3"/>
         <v>33421.926910299007</v>
       </c>
@@ -1214,27 +1265,27 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="8">
         <v>0.34499999999999997</v>
       </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="9">
+        <v>2</v>
+      </c>
+      <c r="C18" s="10">
         <f t="shared" si="4"/>
         <v>2.5874999999999995E-3</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="8">
         <v>11.54</v>
       </c>
-      <c r="E18">
-        <v>20</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="9">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9">
         <f t="shared" si="5"/>
         <v>2.8849999999999997E-2</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="11">
         <f t="shared" si="3"/>
         <v>33449.27536231884</v>
       </c>
@@ -1262,27 +1313,27 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="8">
         <v>0.40100000000000002</v>
       </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10">
         <f t="shared" si="4"/>
         <v>3.0075000000000002E-3</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="8">
         <v>13.41</v>
       </c>
-      <c r="E19">
-        <v>20</v>
-      </c>
-      <c r="F19">
+      <c r="E19" s="9">
+        <v>20</v>
+      </c>
+      <c r="F19" s="9">
         <f t="shared" si="5"/>
         <v>3.3524999999999999E-2</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="11">
         <f t="shared" si="3"/>
         <v>33441.396508728176</v>
       </c>
@@ -1310,27 +1361,27 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="8">
         <v>0.45600000000000002</v>
       </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="9">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10">
         <f t="shared" si="4"/>
         <v>3.4199999999999999E-3</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="8">
         <v>15.23</v>
       </c>
-      <c r="E20">
-        <v>20</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="9">
+        <v>20</v>
+      </c>
+      <c r="F20" s="9">
         <f t="shared" si="5"/>
         <v>3.8075000000000005E-2</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="11">
         <f t="shared" si="3"/>
         <v>33399.122807017542</v>
       </c>
@@ -1358,27 +1409,27 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="8">
         <v>0.51800000000000002</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="9">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10">
         <f t="shared" si="4"/>
         <v>3.885E-3</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="8">
         <v>17.37</v>
       </c>
-      <c r="E21">
-        <v>20</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="9">
+        <v>20</v>
+      </c>
+      <c r="F21" s="9">
         <f t="shared" si="5"/>
         <v>4.3425000000000005E-2</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="11">
         <f t="shared" si="3"/>
         <v>33532.818532818535</v>
       </c>
@@ -1408,27 +1459,27 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="8">
         <v>0.58499999999999996</v>
       </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10">
         <f t="shared" si="4"/>
         <v>4.3874999999999999E-3</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="8">
         <v>19.55</v>
       </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="9">
+        <v>20</v>
+      </c>
+      <c r="F22" s="9">
         <f t="shared" si="5"/>
         <v>4.8875000000000002E-2</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="11">
         <f>D22/(A22/1000)</f>
         <v>33418.803418803422</v>
       </c>
@@ -1444,10 +1495,13 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="2"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
       <c r="P23" s="2">
         <v>1.96</v>
       </c>
@@ -1459,27 +1513,27 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="8">
         <v>1.96</v>
       </c>
-      <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" ref="C24:C33" si="6">MAX(IF(B24=2, 0.001, IF(B24=20, 0.01, IF(B24=200, 0.1))), 0.0075*A24)</f>
+      <c r="B24" s="9">
+        <v>20</v>
+      </c>
+      <c r="C24" s="10">
+        <f>MAX(IF(B24=2, 0.001, IF(B24=20, 0.01, IF(B24=200, 0.1))), 0.0075*A24)</f>
         <v>1.47E-2</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="8">
         <v>1.33</v>
       </c>
-      <c r="E24">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <f t="shared" ref="F24:F33" si="7">MAX(IF(E24=2, 0.001, IF(E24=20, 0.01, IF(E24=200, 0.1))), 0.0025*D24)</f>
+      <c r="E24" s="9">
+        <v>20</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" ref="F24:F33" si="6">MAX(IF(E24=2, 0.001, IF(E24=20, 0.01, IF(E24=200, 0.1))), 0.0025*D24)</f>
         <v>0.01</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="11">
         <f>D24/(A24/1000)</f>
         <v>678.57142857142867</v>
       </c>
@@ -1495,27 +1549,27 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="8">
         <v>7.34</v>
       </c>
-      <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="B25" s="9">
+        <v>20</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" ref="C25:C33" si="7">MAX(IF(B25=2, 0.001, IF(B25=20, 0.01, IF(B25=200, 0.1))), 0.0075*A25)</f>
+        <v>5.5049999999999995E-2</v>
+      </c>
+      <c r="D25" s="8">
+        <v>4.96</v>
+      </c>
+      <c r="E25" s="9">
+        <v>20</v>
+      </c>
+      <c r="F25" s="9">
         <f t="shared" si="6"/>
-        <v>5.5049999999999995E-2</v>
-      </c>
-      <c r="D25" s="2">
-        <v>4.96</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="7"/>
         <v>1.24E-2</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="11">
         <f t="shared" ref="G25:G44" si="8">D25/(A25/1000)</f>
         <v>675.74931880108988</v>
       </c>
@@ -1540,27 +1594,27 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="8">
         <v>8.2200000000000006</v>
       </c>
-      <c r="B26">
-        <v>20</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="B26" s="9">
+        <v>20</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="7"/>
+        <v>6.1650000000000003E-2</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="9">
+        <v>20</v>
+      </c>
+      <c r="F26" s="9">
         <f t="shared" si="6"/>
-        <v>6.1650000000000003E-2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>20</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="7"/>
         <v>1.375E-2</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="11">
         <f t="shared" si="8"/>
         <v>669.09975669099754</v>
       </c>
@@ -1588,27 +1642,27 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="8">
         <v>10.77</v>
       </c>
-      <c r="B27">
-        <v>20</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="B27" s="9">
+        <v>20</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="7"/>
+        <v>8.0775E-2</v>
+      </c>
+      <c r="D27" s="8">
+        <v>7.27</v>
+      </c>
+      <c r="E27" s="9">
+        <v>20</v>
+      </c>
+      <c r="F27" s="9">
         <f t="shared" si="6"/>
-        <v>8.0775E-2</v>
-      </c>
-      <c r="D27" s="2">
-        <v>7.27</v>
-      </c>
-      <c r="E27">
-        <v>20</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="7"/>
         <v>1.8175E-2</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="11">
         <f t="shared" si="8"/>
         <v>675.02321262766941</v>
       </c>
@@ -1624,27 +1678,27 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" s="4">
+      <c r="B28" s="9">
+        <v>20</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="7"/>
+        <v>8.6249999999999993E-2</v>
+      </c>
+      <c r="D28" s="8">
+        <v>7.76</v>
+      </c>
+      <c r="E28" s="9">
+        <v>20</v>
+      </c>
+      <c r="F28" s="9">
         <f t="shared" si="6"/>
-        <v>8.6249999999999993E-2</v>
-      </c>
-      <c r="D28" s="2">
-        <v>7.76</v>
-      </c>
-      <c r="E28">
-        <v>20</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="7"/>
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="11">
         <f t="shared" si="8"/>
         <v>674.78260869565213</v>
       </c>
@@ -1666,27 +1720,27 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="8">
         <v>14.35</v>
       </c>
-      <c r="B29">
-        <v>20</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="B29" s="9">
+        <v>20</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="7"/>
+        <v>0.107625</v>
+      </c>
+      <c r="D29" s="8">
+        <v>9.67</v>
+      </c>
+      <c r="E29" s="9">
+        <v>20</v>
+      </c>
+      <c r="F29" s="9">
         <f t="shared" si="6"/>
-        <v>0.107625</v>
-      </c>
-      <c r="D29" s="2">
-        <v>9.67</v>
-      </c>
-      <c r="E29">
-        <v>20</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="7"/>
         <v>2.4175000000000002E-2</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="11">
         <f t="shared" si="8"/>
         <v>673.86759581881529</v>
       </c>
@@ -1714,27 +1768,27 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="8">
         <v>16.89</v>
       </c>
-      <c r="B30">
-        <v>20</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="B30" s="9">
+        <v>20</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="7"/>
+        <v>0.12667500000000001</v>
+      </c>
+      <c r="D30" s="8">
+        <v>11.38</v>
+      </c>
+      <c r="E30" s="9">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9">
         <f t="shared" si="6"/>
-        <v>0.12667500000000001</v>
-      </c>
-      <c r="D30" s="2">
-        <v>11.38</v>
-      </c>
-      <c r="E30">
-        <v>20</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="7"/>
         <v>2.8450000000000003E-2</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="11">
         <f t="shared" si="8"/>
         <v>673.7714624037892</v>
       </c>
@@ -1762,27 +1816,27 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="8">
         <v>18.55</v>
       </c>
-      <c r="B31">
-        <v>20</v>
-      </c>
-      <c r="C31" s="4">
+      <c r="B31" s="9">
+        <v>20</v>
+      </c>
+      <c r="C31" s="10">
+        <f t="shared" si="7"/>
+        <v>0.139125</v>
+      </c>
+      <c r="D31" s="8">
+        <v>12.45</v>
+      </c>
+      <c r="E31" s="9">
+        <v>20</v>
+      </c>
+      <c r="F31" s="9">
         <f t="shared" si="6"/>
-        <v>0.139125</v>
-      </c>
-      <c r="D31" s="2">
-        <v>12.45</v>
-      </c>
-      <c r="E31">
-        <v>20</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="7"/>
         <v>3.1125E-2</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="11">
         <f t="shared" si="8"/>
         <v>671.1590296495956</v>
       </c>
@@ -1812,27 +1866,27 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="8">
         <v>23.8</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="9">
         <v>200</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="10">
+        <f t="shared" si="7"/>
+        <v>0.17849999999999999</v>
+      </c>
+      <c r="D32" s="8">
+        <v>15.97</v>
+      </c>
+      <c r="E32" s="9">
+        <v>20</v>
+      </c>
+      <c r="F32" s="9">
         <f t="shared" si="6"/>
-        <v>0.17849999999999999</v>
-      </c>
-      <c r="D32" s="2">
-        <v>15.97</v>
-      </c>
-      <c r="E32">
-        <v>20</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="7"/>
         <v>3.9925000000000002E-2</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="11">
         <f t="shared" si="8"/>
         <v>671.00840336134456</v>
       </c>
@@ -1862,27 +1916,27 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="A33" s="8">
         <v>26.2</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="9">
         <v>200</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="10">
+        <f t="shared" si="7"/>
+        <v>0.19649999999999998</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="9">
+        <v>20</v>
+      </c>
+      <c r="F33" s="9">
         <f t="shared" si="6"/>
-        <v>0.19649999999999998</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33">
-        <v>20</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="7"/>
         <v>4.3750000000000004E-2</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="11">
         <f t="shared" si="8"/>
         <v>667.93893129771004</v>
       </c>
@@ -1898,6 +1952,13 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
       <c r="P34" s="2">
         <v>0.67500000000000004</v>
       </c>
@@ -1909,27 +1970,27 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="A35" s="8">
         <v>0.51800000000000002</v>
       </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B35" s="9">
+        <v>2</v>
+      </c>
+      <c r="C35" s="10">
         <f t="shared" ref="C35:C44" si="9">MAX(IF(B35=2, 0.001, IF(B35=20, 0.01, IF(B35=200, 0.1))), 0.0075*A35)</f>
         <v>3.885E-3</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="8">
         <v>4.34</v>
       </c>
-      <c r="E35">
-        <v>20</v>
-      </c>
-      <c r="F35">
+      <c r="E35" s="9">
+        <v>20</v>
+      </c>
+      <c r="F35" s="9">
         <f t="shared" ref="F35:F44" si="10">MAX(IF(E35=2, 0.001, IF(E35=20, 0.01, IF(E35=200, 0.1))), 0.0025*D35)</f>
         <v>1.085E-2</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="11">
         <f t="shared" si="8"/>
         <v>8378.3783783783783</v>
       </c>
@@ -1945,27 +2006,27 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="A36" s="8">
         <v>0.67500000000000004</v>
       </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="B36" s="9">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10">
         <f t="shared" si="9"/>
         <v>5.0625000000000002E-3</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="8">
         <v>5.58</v>
       </c>
-      <c r="E36">
-        <v>20</v>
-      </c>
-      <c r="F36">
+      <c r="E36" s="9">
+        <v>20</v>
+      </c>
+      <c r="F36" s="9">
         <f t="shared" si="10"/>
         <v>1.3950000000000001E-2</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="11">
         <f t="shared" si="8"/>
         <v>8266.6666666666661</v>
       </c>
@@ -1990,27 +2051,27 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="A37" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" s="4">
+      <c r="B37" s="9">
+        <v>2</v>
+      </c>
+      <c r="C37" s="10">
         <f t="shared" si="9"/>
         <v>5.8875000000000004E-3</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="8">
         <v>6.49</v>
       </c>
-      <c r="E37">
-        <v>20</v>
-      </c>
-      <c r="F37">
+      <c r="E37" s="9">
+        <v>20</v>
+      </c>
+      <c r="F37" s="9">
         <f t="shared" si="10"/>
         <v>1.6225E-2</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="11">
         <f t="shared" si="8"/>
         <v>8267.5159235668798</v>
       </c>
@@ -2038,27 +2099,27 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="A38" s="8">
         <v>0.92600000000000005</v>
       </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" s="4">
+      <c r="B38" s="9">
+        <v>2</v>
+      </c>
+      <c r="C38" s="10">
         <f t="shared" si="9"/>
         <v>6.9449999999999998E-3</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="8">
         <v>7.65</v>
       </c>
-      <c r="E38">
-        <v>20</v>
-      </c>
-      <c r="F38">
+      <c r="E38" s="9">
+        <v>20</v>
+      </c>
+      <c r="F38" s="9">
         <f t="shared" si="10"/>
         <v>1.9125E-2</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="11">
         <f t="shared" si="8"/>
         <v>8261.3390928725694</v>
       </c>
@@ -2074,27 +2135,27 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" s="4">
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10">
         <f t="shared" si="9"/>
         <v>7.9500000000000005E-3</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="8">
         <v>8.77</v>
       </c>
-      <c r="E39">
-        <v>20</v>
-      </c>
-      <c r="F39">
+      <c r="E39" s="9">
+        <v>20</v>
+      </c>
+      <c r="F39" s="9">
         <f t="shared" si="10"/>
         <v>2.1925E-2</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="11">
         <f t="shared" si="8"/>
         <v>8273.5849056603765</v>
       </c>
@@ -2116,27 +2177,27 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="A40" s="8">
         <v>1.3819999999999999</v>
       </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="B40" s="9">
+        <v>2</v>
+      </c>
+      <c r="C40" s="10">
         <f t="shared" si="9"/>
         <v>1.0364999999999999E-2</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="8">
         <v>11.43</v>
       </c>
-      <c r="E40">
-        <v>20</v>
-      </c>
-      <c r="F40">
+      <c r="E40" s="9">
+        <v>20</v>
+      </c>
+      <c r="F40" s="9">
         <f t="shared" si="10"/>
         <v>2.8575E-2</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="11">
         <f t="shared" si="8"/>
         <v>8270.6222865412437</v>
       </c>
@@ -2164,27 +2225,27 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="A41" s="8">
         <v>1.448</v>
       </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="B41" s="9">
+        <v>2</v>
+      </c>
+      <c r="C41" s="10">
         <f t="shared" si="9"/>
         <v>1.086E-2</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="8">
         <v>11.97</v>
       </c>
-      <c r="E41">
-        <v>20</v>
-      </c>
-      <c r="F41">
+      <c r="E41" s="9">
+        <v>20</v>
+      </c>
+      <c r="F41" s="9">
         <f t="shared" si="10"/>
         <v>2.9925000000000004E-2</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="11">
         <f t="shared" si="8"/>
         <v>8266.5745856353606</v>
       </c>
@@ -2212,27 +2273,27 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="A42" s="8">
         <v>1.6659999999999999</v>
       </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="B42" s="9">
+        <v>2</v>
+      </c>
+      <c r="C42" s="10">
         <f t="shared" si="9"/>
         <v>1.2494999999999999E-2</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="8">
         <v>13.78</v>
       </c>
-      <c r="E42">
-        <v>20</v>
-      </c>
-      <c r="F42">
+      <c r="E42" s="9">
+        <v>20</v>
+      </c>
+      <c r="F42" s="9">
         <f t="shared" si="10"/>
         <v>3.4450000000000001E-2</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="11">
         <f t="shared" si="8"/>
         <v>8271.3085234093633</v>
       </c>
@@ -2262,27 +2323,27 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="A43" s="8">
         <v>1.869</v>
       </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="B43" s="9">
+        <v>2</v>
+      </c>
+      <c r="C43" s="10">
         <f t="shared" si="9"/>
         <v>1.4017499999999999E-2</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="8">
         <v>15.48</v>
       </c>
-      <c r="E43">
-        <v>20</v>
-      </c>
-      <c r="F43">
+      <c r="E43" s="9">
+        <v>20</v>
+      </c>
+      <c r="F43" s="9">
         <f t="shared" si="10"/>
         <v>3.8700000000000005E-2</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="11">
         <f t="shared" si="8"/>
         <v>8282.504012841091</v>
       </c>
@@ -2303,27 +2364,27 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="A44" s="8">
         <v>2.13</v>
       </c>
-      <c r="B44">
-        <v>20</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="B44" s="9">
+        <v>20</v>
+      </c>
+      <c r="C44" s="10">
         <f t="shared" si="9"/>
         <v>1.5975E-2</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E44">
-        <v>20</v>
-      </c>
-      <c r="F44">
+      <c r="E44" s="9">
+        <v>20</v>
+      </c>
+      <c r="F44" s="9">
         <f t="shared" si="10"/>
         <v>4.4000000000000004E-2</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="11">
         <f t="shared" si="8"/>
         <v>8262.9107981220659</v>
       </c>
@@ -2342,6 +2403,671 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3A25E8-52BB-B943-AAFA-71CEFFE3FB32}">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="F43" sqref="A1:F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>1.373</v>
+      </c>
+      <c r="C1" s="4">
+        <f t="shared" ref="C1:C10" si="0">MAX(IF(B1=2, 0.001, IF(B1=20, 0.01, IF(B1=200, 0.1))), 0.0075*A1)</f>
+        <v>1.0297499999999999E-2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="F1">
+        <f t="shared" ref="F1:F10" si="1">MAX(IF(E1=2, 0.001, IF(E1=20, 0.01, IF(E1=200, 0.1))), 0.0025*D1)</f>
+        <v>2.8050000000000002E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>3.81</v>
+      </c>
+      <c r="C2" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8575E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="1"/>
+        <v>7.7749999999999998E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" si="0"/>
+        <v>4.725E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.12</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>1.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>5.1150000000000001E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.53</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1.3825E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>9.36</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>7.0199999999999999E-2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>9.49</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>7.1175000000000002E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.72</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.9300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>14.22</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.10664999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11.56</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2.8900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>15.57</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.116775</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12.67</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>3.1675000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>17.07</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.128025</v>
+      </c>
+      <c r="D9" s="2">
+        <v>13.83</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3.4575000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>19.36</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1452</v>
+      </c>
+      <c r="D10" s="2">
+        <v>15.64</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.9100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:C21" si="2">MAX(IF(B12=2, 0.001, IF(B12=20, 0.01, IF(B12=200, 0.1))), 0.0075*A12)</f>
+        <v>9.8250000000000008E-4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F21" si="3">MAX(IF(E12=2, 0.001, IF(E12=20, 0.01, IF(E12=200, 0.1))), 0.0025*D12)</f>
+        <v>1.1050000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="2"/>
+        <v>1.2750000000000001E-3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.57</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>1.3925000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>0.187</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="2"/>
+        <v>1.4024999999999999E-3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>1.5575000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="2"/>
+        <v>1.74E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7.74</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>1.9350000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2575E-3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10.06</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>2.5150000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5874999999999995E-3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>11.54</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>2.8849999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="2"/>
+        <v>3.0075000000000002E-3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>13.41</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>3.3524999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="2"/>
+        <v>3.4199999999999999E-3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>15.23</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>3.8075000000000005E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="2"/>
+        <v>3.885E-3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>17.37</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>4.3425000000000005E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="2"/>
+        <v>4.3874999999999999E-3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>19.55</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>4.8875000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:C32" si="4">MAX(IF(B23=2, 0.001, IF(B23=20, 0.01, IF(B23=200, 0.1))), 0.0075*A23)</f>
+        <v>1.47E-2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23:F32" si="5">MAX(IF(E23=2, 0.001, IF(E23=20, 0.01, IF(E23=200, 0.1))), 0.0025*D23)</f>
+        <v>3.3250000000000003E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>7.34</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="4"/>
+        <v>5.5049999999999995E-2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.96</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="4"/>
+        <v>6.1650000000000003E-2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="5"/>
+        <v>1.375E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>10.77</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="4"/>
+        <v>8.0775E-2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>1.8175E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="4"/>
+        <v>8.6249999999999993E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>7.76</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>1.9400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>14.35</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="4"/>
+        <v>0.107625</v>
+      </c>
+      <c r="D28" s="2">
+        <v>9.67</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>2.4175000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>16.89</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="4"/>
+        <v>0.12667500000000001</v>
+      </c>
+      <c r="D29" s="2">
+        <v>11.38</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>2.8450000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>18.55</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="4"/>
+        <v>0.139125</v>
+      </c>
+      <c r="D30" s="2">
+        <v>12.45</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="5"/>
+        <v>3.1125E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17849999999999999</v>
+      </c>
+      <c r="D31" s="2">
+        <v>15.97</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="5"/>
+        <v>3.9925000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19649999999999998</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>4.3750000000000004E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" ref="C34:C43" si="6">MAX(IF(B34=2, 0.001, IF(B34=20, 0.01, IF(B34=200, 0.1))), 0.0075*A34)</f>
+        <v>3.885E-3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.34</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F43" si="7">MAX(IF(E34=2, 0.001, IF(E34=20, 0.01, IF(E34=200, 0.1))), 0.0025*D34)</f>
+        <v>1.085E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="6"/>
+        <v>5.0625000000000002E-3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5.58</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="7"/>
+        <v>1.3950000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="6"/>
+        <v>5.8875000000000004E-3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>6.49</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="7"/>
+        <v>1.6225E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="6"/>
+        <v>6.9449999999999998E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7.65</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="7"/>
+        <v>1.9125E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="6"/>
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>8.77</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="7"/>
+        <v>2.1925E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1.3819999999999999</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0364999999999999E-2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>11.43</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="7"/>
+        <v>2.8575E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>1.448</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="6"/>
+        <v>1.086E-2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>11.97</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="7"/>
+        <v>2.9925000000000004E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="6"/>
+        <v>1.2494999999999999E-2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>13.78</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="7"/>
+        <v>3.4450000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>1.869</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="6"/>
+        <v>1.4017499999999999E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>15.48</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="7"/>
+        <v>3.8700000000000005E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>2.13</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="6"/>
+        <v>1.5975E-2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="7"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7548BC-6D4C-8041-9570-DA2E9C9D80FF}">
   <dimension ref="A1:C40"/>
   <sheetViews>
@@ -2796,7 +3522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9FA899-4D84-6343-BA2A-7F0ADCCB1FAD}">
   <dimension ref="A1:C40"/>
   <sheetViews>

</xml_diff>